<commit_message>
Modelo das pastas corriers
</commit_message>
<xml_diff>
--- a/Document/Backlog.xlsx
+++ b/Document/Backlog.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
+    <sheet name="Color Match Request" sheetId="2" r:id="rId2"/>
+    <sheet name="Plan2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -919,8 +921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -946,22 +948,32 @@
       <c r="A3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="12"/>
+      <c r="B3" s="11">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="4"/>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
@@ -981,7 +993,9 @@
       <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
       <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1017,7 +1031,9 @@
       <c r="A13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
       <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -1052,7 +1068,9 @@
       <c r="A18" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
       <c r="C18" s="4"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -1797,4 +1815,32 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>